<commit_message>
Upd reports, start plot report
</commit_message>
<xml_diff>
--- a/reports/annotation_results_rede_1.xlsx
+++ b/reports/annotation_results_rede_1.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\Arquivos Incomuns\Projeto Final\semiauto-video-annotation\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40841780-D482-4AF0-AB5C-0F3BD833FCC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B529F8C3-0E1E-45FF-85B1-1BD04830F42F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,8 +33,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={9D51D838-F358-4BEA-BCA5-AE160B6AF3E0}</author>
+  </authors>
+  <commentList>
+    <comment ref="J13" authorId="0" shapeId="0" xr:uid="{9D51D838-F358-4BEA-BCA5-AE160B6AF3E0}">
+      <text>
+        <t>[Comentário encadeado]
+Sua versão do Excel permite que você leia este comentário encadeado, no entanto, as edições serão removidas se o arquivo for aberto em uma versão mais recente do Excel. Saiba mais: https://go.microsoft.com/fwlink/?linkid=870924
+Comentário:
+    maior que 100% por cause de imagens duplicadas no primeiro conjunto de anotações manuais</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>manual</t>
   </si>
@@ -76,12 +95,39 @@
   <si>
     <t>rede3</t>
   </si>
+  <si>
+    <t>% manual relative</t>
+  </si>
+  <si>
+    <t>% automatic relative</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>auto</t>
+  </si>
+  <si>
+    <t>% auto</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>It</t>
+  </si>
+  <si>
+    <t>% unlabeled</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,16 +135,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -106,19 +166,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="11">
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
@@ -152,9 +238,6 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -166,6 +249,919 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Unlabeled % x Iteration</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Plan1!$K$23:$K$32</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.6228015707126802E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.8851438216593929E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.2210716878164821E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.3827431499960645E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.7937258948951838E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.022581181182932E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2064577630462731E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.815581189928548E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-38A1-44C9-80FA-90AAB924B3EA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1197997744"/>
+        <c:axId val="1369001856"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1197997744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1369001856"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1369001856"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1197997744"/>
+        <c:crossesAt val="1"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>301624</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>6349</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD7B7669-D8A2-4409-9375-D01282BCC7A3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Olavo Sampaio" id="{7DC51EB1-0F23-494A-90AB-5A5E6854DE42}" userId="5dc859e3f5210d34" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -182,9 +1178,12 @@
     <tableColumn id="9" xr3:uid="{DE24A7CD-C95D-43B4-A9E9-E3AC9E362224}" name="unlabeled" totalsRowFunction="custom">
       <totalsRowFormula>Tabela1[[#Totals],[manual]]+Tabela1[[#Totals],[automatic]]</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{A9E70562-3FA3-48EF-9795-59254BDFF23F}" name="unlabeled real"/>
-    <tableColumn id="13" xr3:uid="{F6CC74BF-52DF-4FEE-860E-97C47DA93CFD}" name="diff" dataDxfId="11" totalsRowDxfId="10">
+    <tableColumn id="12" xr3:uid="{A9E70562-3FA3-48EF-9795-59254BDFF23F}" name="unlabeled real" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Tabela1[unlabeled real])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="13" xr3:uid="{F6CC74BF-52DF-4FEE-860E-97C47DA93CFD}" name="diff" totalsRowFunction="custom" dataDxfId="10">
       <calculatedColumnFormula>Tabela1[[#This Row],[unlabeled real]]-Tabela1[[#This Row],[unlabeled]]</calculatedColumnFormula>
+      <totalsRowFormula>SUM(Tabela1[diff])</totalsRowFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{7739FE3C-1F66-4C35-AFB6-BFAEB1B69C1F}" name="% manual" dataDxfId="9" totalsRowDxfId="8">
       <calculatedColumnFormula>Tabela1[[#This Row],[manual]]/E2</calculatedColumnFormula>
@@ -465,17 +1464,25 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="J13" dT="2020-02-07T15:55:21.73" personId="{7DC51EB1-0F23-494A-90AB-5A5E6854DE42}" id="{9D51D838-F358-4BEA-BCA5-AE160B6AF3E0}">
+    <text>maior que 100% por cause de imagens duplicadas no primeiro conjunto de anotações manuais</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:M18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="3.7265625" customWidth="1"/>
+    <col min="2" max="2" width="5.08984375" customWidth="1"/>
     <col min="3" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.6328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.6328125" customWidth="1"/>
@@ -547,17 +1554,17 @@
         <f>Tabela1[[#This Row],[unlabeled real]]-Tabela1[[#This Row],[unlabeled]]</f>
         <v>0</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="1">
         <v>0</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="1">
         <v>0</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="1">
         <v>0</v>
       </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B4">
@@ -580,20 +1587,20 @@
         <f>Tabela1[[#This Row],[unlabeled real]]-Tabela1[[#This Row],[unlabeled]]</f>
         <v>2</v>
       </c>
-      <c r="H4" s="2">
-        <f>Tabela1[[#This Row],[manual]]/F3</f>
+      <c r="H4" s="1">
+        <f>Tabela1[[#This Row],[manual]]/E3</f>
         <v>1.0221439003699396E-2</v>
       </c>
-      <c r="I4" s="2">
-        <f>Tabela1[[#This Row],[automatic]]/F3</f>
+      <c r="I4" s="1">
+        <f>Tabela1[[#This Row],[automatic]]/E3</f>
         <v>0.8935549180973037</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="1">
         <f>(Tabela1[[#This Row],[manual]]+Tabela1[[#This Row],[automatic]])/$E$3</f>
         <v>0.90377635710100312</v>
       </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B5">
@@ -616,20 +1623,20 @@
         <f>Tabela1[[#This Row],[unlabeled real]]-Tabela1[[#This Row],[unlabeled]]</f>
         <v>191</v>
       </c>
-      <c r="H5" s="2">
-        <f>Tabela1[[#This Row],[manual]]/F4</f>
-        <v>9.9972734708715805E-3</v>
-      </c>
-      <c r="I5" s="2">
-        <f>Tabela1[[#This Row],[automatic]]/F4</f>
-        <v>0.38271380532582022</v>
-      </c>
-      <c r="J5" s="2">
+      <c r="H5" s="1">
+        <f>Tabela1[[#This Row],[manual]]/E4</f>
+        <v>9.9977277891388321E-3</v>
+      </c>
+      <c r="I5" s="1">
+        <f>Tabela1[[#This Row],[automatic]]/E4</f>
+        <v>0.38273119745512385</v>
+      </c>
+      <c r="J5" s="1">
         <f>(Tabela1[[#This Row],[manual]]+Tabela1[[#This Row],[automatic]])/$E$3</f>
         <v>3.7789807858810774E-2</v>
       </c>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B6">
@@ -652,20 +1659,20 @@
         <f>Tabela1[[#This Row],[unlabeled real]]-Tabela1[[#This Row],[unlabeled]]</f>
         <v>259</v>
       </c>
-      <c r="H6" s="2">
-        <f>Tabela1[[#This Row],[manual]]/F5</f>
-        <v>9.9936842887394586E-3</v>
-      </c>
-      <c r="I6" s="2">
-        <f>Tabela1[[#This Row],[automatic]]/F5</f>
-        <v>0.27529070847419845</v>
-      </c>
-      <c r="J6" s="2">
+      <c r="H6" s="1">
+        <f>Tabela1[[#This Row],[manual]]/E5</f>
+        <v>1.006510514106114E-2</v>
+      </c>
+      <c r="I6" s="1">
+        <f>Tabela1[[#This Row],[automatic]]/E5</f>
+        <v>0.27725810072588492</v>
+      </c>
+      <c r="J6" s="1">
         <f>(Tabela1[[#This Row],[manual]]+Tabela1[[#This Row],[automatic]])/$E$3</f>
         <v>1.678939681484656E-2</v>
       </c>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B7">
@@ -688,20 +1695,20 @@
         <f>Tabela1[[#This Row],[unlabeled real]]-Tabela1[[#This Row],[unlabeled]]</f>
         <v>363</v>
       </c>
-      <c r="H7" s="2">
-        <f>Tabela1[[#This Row],[manual]]/F6</f>
-        <v>9.9968921578783791E-3</v>
-      </c>
-      <c r="I7" s="2">
-        <f>Tabela1[[#This Row],[automatic]]/F6</f>
-        <v>0.43090231016264374</v>
-      </c>
-      <c r="J7" s="2">
+      <c r="H7" s="1">
+        <f>Tabela1[[#This Row],[manual]]/E6</f>
+        <v>1.01328293169528E-2</v>
+      </c>
+      <c r="I7" s="1">
+        <f>Tabela1[[#This Row],[automatic]]/E6</f>
+        <v>0.43676169475507953</v>
+      </c>
+      <c r="J7" s="1">
         <f>(Tabela1[[#This Row],[manual]]+Tabela1[[#This Row],[automatic]])/$E$3</f>
         <v>1.8610671400960267E-2</v>
       </c>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B8">
@@ -724,20 +1731,20 @@
         <f>Tabela1[[#This Row],[unlabeled real]]-Tabela1[[#This Row],[unlabeled]]</f>
         <v>395</v>
       </c>
-      <c r="H8" s="2">
-        <f>Tabela1[[#This Row],[manual]]/F7</f>
-        <v>9.910075243163884E-3</v>
-      </c>
-      <c r="I8" s="2">
-        <f>Tabela1[[#This Row],[automatic]]/F7</f>
-        <v>0.24022756469076895</v>
-      </c>
-      <c r="J8" s="2">
+      <c r="H8" s="1">
+        <f>Tabela1[[#This Row],[manual]]/E7</f>
+        <v>1.0251542477456098E-2</v>
+      </c>
+      <c r="I8" s="1">
+        <f>Tabela1[[#This Row],[automatic]]/E7</f>
+        <v>0.24850498338870433</v>
+      </c>
+      <c r="J8" s="1">
         <f>(Tabela1[[#This Row],[manual]]+Tabela1[[#This Row],[automatic]])/$E$3</f>
         <v>5.9601374810876045E-3</v>
       </c>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B9">
@@ -760,20 +1767,20 @@
         <f>Tabela1[[#This Row],[unlabeled real]]-Tabela1[[#This Row],[unlabeled]]</f>
         <v>-1371</v>
       </c>
-      <c r="H9" s="2">
-        <f>Tabela1[[#This Row],[manual]]/F8</f>
-        <v>1.218917601170161E-2</v>
-      </c>
-      <c r="I9" s="2">
-        <f>Tabela1[[#This Row],[automatic]]/F8</f>
-        <v>0.20246221355436372</v>
-      </c>
-      <c r="J9" s="2">
+      <c r="H9" s="1">
+        <f>Tabela1[[#This Row],[manual]]/E8</f>
+        <v>1.2805736970162632E-2</v>
+      </c>
+      <c r="I9" s="1">
+        <f>Tabela1[[#This Row],[automatic]]/E8</f>
+        <v>0.21270329107440133</v>
+      </c>
+      <c r="J9" s="1">
         <f>(Tabela1[[#This Row],[manual]]+Tabela1[[#This Row],[automatic]])/$E$3</f>
         <v>3.8502575583988525E-3</v>
       </c>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B10">
@@ -796,20 +1803,20 @@
         <f>Tabela1[[#This Row],[unlabeled real]]-Tabela1[[#This Row],[unlabeled]]</f>
         <v>442</v>
       </c>
-      <c r="H10" s="2">
-        <f>Tabela1[[#This Row],[manual]]/F9</f>
-        <v>2.1381227282446014E-2</v>
-      </c>
-      <c r="I10" s="2">
-        <f>Tabela1[[#This Row],[automatic]]/F9</f>
-        <v>0.18644430190292924</v>
-      </c>
-      <c r="J10" s="2">
+      <c r="H10" s="1">
+        <f>Tabela1[[#This Row],[manual]]/E9</f>
+        <v>1.6534391534391533E-2</v>
+      </c>
+      <c r="I10" s="1">
+        <f>Tabela1[[#This Row],[automatic]]/E9</f>
+        <v>0.14417989417989419</v>
+      </c>
+      <c r="J10" s="1">
         <f>(Tabela1[[#This Row],[manual]]+Tabela1[[#This Row],[automatic]])/$E$3</f>
         <v>2.1251847511434894E-3</v>
       </c>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B11">
@@ -832,20 +1839,20 @@
         <f>Tabela1[[#This Row],[unlabeled real]]-Tabela1[[#This Row],[unlabeled]]</f>
         <v>484</v>
       </c>
-      <c r="H11" s="2">
-        <f>Tabela1[[#This Row],[manual]]/F10</f>
-        <v>1.8122508155128669E-2</v>
-      </c>
-      <c r="I11" s="2">
-        <f>Tabela1[[#This Row],[automatic]]/F10</f>
-        <v>0.2587894164552374</v>
-      </c>
-      <c r="J11" s="2">
+      <c r="H11" s="1">
+        <f>Tabela1[[#This Row],[manual]]/E10</f>
+        <v>1.9700551615445233E-2</v>
+      </c>
+      <c r="I11" s="1">
+        <f>Tabela1[[#This Row],[automatic]]/E10</f>
+        <v>0.28132387706855794</v>
+      </c>
+      <c r="J11" s="1">
         <f>(Tabela1[[#This Row],[manual]]+Tabela1[[#This Row],[automatic]])/$E$3</f>
         <v>3.3408254112626047E-3</v>
       </c>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B12">
@@ -868,20 +1875,20 @@
         <f>Tabela1[[#This Row],[unlabeled real]]-Tabela1[[#This Row],[unlabeled]]</f>
         <v>483</v>
       </c>
-      <c r="H12" s="2">
-        <f>Tabela1[[#This Row],[manual]]/F11</f>
-        <v>0.99975198412698407</v>
-      </c>
-      <c r="I12" s="2">
-        <f>Tabela1[[#This Row],[automatic]]/F11</f>
+      <c r="H12" s="1">
+        <f>Tabela1[[#This Row],[manual]]/E11</f>
+        <v>1.1361330326944759</v>
+      </c>
+      <c r="I12" s="1">
+        <f>Tabela1[[#This Row],[automatic]]/E11</f>
         <v>0</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="1">
         <f>(Tabela1[[#This Row],[manual]]+Tabela1[[#This Row],[automatic]])/$E$3</f>
         <v>8.8133947858635864E-3</v>
       </c>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C13">
@@ -896,18 +1903,25 @@
         <f>Tabela1[[#Totals],[manual]]+Tabela1[[#Totals],[automatic]]</f>
         <v>457855</v>
       </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2">
+      <c r="F13">
+        <f>SUM(Tabela1[unlabeled real])</f>
+        <v>580936</v>
+      </c>
+      <c r="G13">
+        <f>SUM(Tabela1[diff])</f>
+        <v>1248</v>
+      </c>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1">
         <f>SUM(Tabela1[% annotated])</f>
         <v>1.0010560331633769</v>
       </c>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="K14" s="2">
+      <c r="K14" s="1">
         <f>SUM(J5:J12)</f>
         <v>9.7279676062373727E-2</v>
       </c>
@@ -920,7 +1934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.35">
       <c r="H17" t="s">
         <v>13</v>
       </c>
@@ -928,17 +1942,480 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.35">
       <c r="I18">
         <f>6*9</f>
         <v>54</v>
       </c>
     </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="K22" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B23" s="10">
+        <v>0</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
+      <c r="E23" s="3">
+        <v>457372</v>
+      </c>
+      <c r="F23" s="5">
+        <v>0</v>
+      </c>
+      <c r="G23" s="5">
+        <v>0</v>
+      </c>
+      <c r="H23" s="5">
+        <v>0</v>
+      </c>
+      <c r="I23" s="5">
+        <v>0</v>
+      </c>
+      <c r="J23" s="5">
+        <v>0</v>
+      </c>
+      <c r="K23" s="1">
+        <f>E23/E$23</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B24" s="11">
+        <v>1</v>
+      </c>
+      <c r="C24" s="4">
+        <v>4675</v>
+      </c>
+      <c r="D24" s="4">
+        <v>408687</v>
+      </c>
+      <c r="E24" s="4">
+        <v>44012</v>
+      </c>
+      <c r="F24" s="6">
+        <f>C24/$E$23</f>
+        <v>1.0221439003699396E-2</v>
+      </c>
+      <c r="G24" s="6">
+        <f>D24/$E$23</f>
+        <v>0.8935549180973037</v>
+      </c>
+      <c r="H24" s="6">
+        <f>(C24+D24)/$E$23</f>
+        <v>0.90377635710100312</v>
+      </c>
+      <c r="I24" s="1">
+        <f>C24/E23</f>
+        <v>1.0221439003699396E-2</v>
+      </c>
+      <c r="J24" s="1">
+        <f>D24/E23</f>
+        <v>0.8935549180973037</v>
+      </c>
+      <c r="K24" s="1">
+        <f t="shared" ref="K24:K32" si="0">E24/E$23</f>
+        <v>9.6228015707126802E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B25" s="10">
+        <v>2</v>
+      </c>
+      <c r="C25" s="3">
+        <v>440</v>
+      </c>
+      <c r="D25" s="3">
+        <v>16844</v>
+      </c>
+      <c r="E25" s="3">
+        <v>26917</v>
+      </c>
+      <c r="F25" s="6">
+        <f t="shared" ref="F25:F31" si="1">C25/$E$23</f>
+        <v>9.6201778858347252E-4</v>
+      </c>
+      <c r="G25" s="6">
+        <f t="shared" ref="G25:G32" si="2">D25/$E$23</f>
+        <v>3.6827790070227295E-2</v>
+      </c>
+      <c r="H25" s="6">
+        <f t="shared" ref="H25:H32" si="3">(C25+D25)/$E$23</f>
+        <v>3.7789807858810774E-2</v>
+      </c>
+      <c r="I25" s="1">
+        <f t="shared" ref="I25:I32" si="4">C25/E24</f>
+        <v>9.9972734708715805E-3</v>
+      </c>
+      <c r="J25" s="1">
+        <f t="shared" ref="J25:J32" si="5">D25/E24</f>
+        <v>0.38271380532582022</v>
+      </c>
+      <c r="K25" s="1">
+        <f t="shared" si="0"/>
+        <v>5.8851438216593929E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B26" s="11">
+        <v>3</v>
+      </c>
+      <c r="C26" s="4">
+        <v>269</v>
+      </c>
+      <c r="D26" s="4">
+        <v>7410</v>
+      </c>
+      <c r="E26" s="4">
+        <v>19306</v>
+      </c>
+      <c r="F26" s="6">
+        <f t="shared" si="1"/>
+        <v>5.8814269347489572E-4</v>
+      </c>
+      <c r="G26" s="6">
+        <f t="shared" si="2"/>
+        <v>1.6201254121371661E-2</v>
+      </c>
+      <c r="H26" s="6">
+        <f t="shared" si="3"/>
+        <v>1.678939681484656E-2</v>
+      </c>
+      <c r="I26" s="1">
+        <f t="shared" si="4"/>
+        <v>9.9936842887394586E-3</v>
+      </c>
+      <c r="J26" s="1">
+        <f t="shared" si="5"/>
+        <v>0.27529070847419845</v>
+      </c>
+      <c r="K26" s="1">
+        <f t="shared" si="0"/>
+        <v>4.2210716878164821E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B27" s="10">
+        <v>4</v>
+      </c>
+      <c r="C27" s="3">
+        <v>193</v>
+      </c>
+      <c r="D27" s="3">
+        <v>8319</v>
+      </c>
+      <c r="E27" s="3">
+        <v>10898</v>
+      </c>
+      <c r="F27" s="6">
+        <f t="shared" si="1"/>
+        <v>4.2197598453775048E-4</v>
+      </c>
+      <c r="G27" s="6">
+        <f t="shared" si="2"/>
+        <v>1.8188695416422519E-2</v>
+      </c>
+      <c r="H27" s="6">
+        <f t="shared" si="3"/>
+        <v>1.8610671400960267E-2</v>
+      </c>
+      <c r="I27" s="1">
+        <f t="shared" si="4"/>
+        <v>9.9968921578783791E-3</v>
+      </c>
+      <c r="J27" s="1">
+        <f t="shared" si="5"/>
+        <v>0.43090231016264374</v>
+      </c>
+      <c r="K27" s="1">
+        <f t="shared" si="0"/>
+        <v>2.3827431499960645E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B28" s="11">
+        <v>5</v>
+      </c>
+      <c r="C28" s="4">
+        <v>108</v>
+      </c>
+      <c r="D28" s="4">
+        <v>2618</v>
+      </c>
+      <c r="E28" s="4">
+        <v>8204</v>
+      </c>
+      <c r="F28" s="6">
+        <f t="shared" si="1"/>
+        <v>2.3613163901594326E-4</v>
+      </c>
+      <c r="G28" s="6">
+        <f t="shared" si="2"/>
+        <v>5.7240058420716614E-3</v>
+      </c>
+      <c r="H28" s="6">
+        <f t="shared" si="3"/>
+        <v>5.9601374810876045E-3</v>
+      </c>
+      <c r="I28" s="1">
+        <f t="shared" si="4"/>
+        <v>9.910075243163884E-3</v>
+      </c>
+      <c r="J28" s="1">
+        <f t="shared" si="5"/>
+        <v>0.24022756469076895</v>
+      </c>
+      <c r="K28" s="1">
+        <f t="shared" si="0"/>
+        <v>1.7937258948951838E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B29" s="10">
+        <v>6</v>
+      </c>
+      <c r="C29" s="3">
+        <v>100</v>
+      </c>
+      <c r="D29" s="3">
+        <v>1661</v>
+      </c>
+      <c r="E29" s="3">
+        <v>4677</v>
+      </c>
+      <c r="F29" s="6">
+        <f t="shared" si="1"/>
+        <v>2.1864040649624376E-4</v>
+      </c>
+      <c r="G29" s="6">
+        <f t="shared" si="2"/>
+        <v>3.6316171519026087E-3</v>
+      </c>
+      <c r="H29" s="6">
+        <f t="shared" si="3"/>
+        <v>3.8502575583988525E-3</v>
+      </c>
+      <c r="I29" s="1">
+        <f t="shared" si="4"/>
+        <v>1.218917601170161E-2</v>
+      </c>
+      <c r="J29" s="1">
+        <f t="shared" si="5"/>
+        <v>0.20246221355436372</v>
+      </c>
+      <c r="K29" s="1">
+        <f t="shared" si="0"/>
+        <v>1.022581181182932E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B30" s="11">
+        <v>7</v>
+      </c>
+      <c r="C30" s="4">
+        <v>100</v>
+      </c>
+      <c r="D30" s="4">
+        <v>872</v>
+      </c>
+      <c r="E30" s="4">
+        <v>5518</v>
+      </c>
+      <c r="F30" s="6">
+        <f t="shared" si="1"/>
+        <v>2.1864040649624376E-4</v>
+      </c>
+      <c r="G30" s="6">
+        <f t="shared" si="2"/>
+        <v>1.9065443446472457E-3</v>
+      </c>
+      <c r="H30" s="6">
+        <f t="shared" si="3"/>
+        <v>2.1251847511434894E-3</v>
+      </c>
+      <c r="I30" s="1">
+        <f t="shared" si="4"/>
+        <v>2.1381227282446014E-2</v>
+      </c>
+      <c r="J30" s="1">
+        <f t="shared" si="5"/>
+        <v>0.18644430190292924</v>
+      </c>
+      <c r="K30" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2064577630462731E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B31" s="10">
+        <v>8</v>
+      </c>
+      <c r="C31" s="3">
+        <v>100</v>
+      </c>
+      <c r="D31" s="3">
+        <v>1428</v>
+      </c>
+      <c r="E31" s="3">
+        <v>4032</v>
+      </c>
+      <c r="F31" s="6">
+        <f t="shared" si="1"/>
+        <v>2.1864040649624376E-4</v>
+      </c>
+      <c r="G31" s="6">
+        <f t="shared" si="2"/>
+        <v>3.1221850047663609E-3</v>
+      </c>
+      <c r="H31" s="6">
+        <f t="shared" si="3"/>
+        <v>3.3408254112626047E-3</v>
+      </c>
+      <c r="I31" s="1">
+        <f t="shared" si="4"/>
+        <v>1.8122508155128669E-2</v>
+      </c>
+      <c r="J31" s="1">
+        <f t="shared" si="5"/>
+        <v>0.2587894164552374</v>
+      </c>
+      <c r="K31" s="1">
+        <f t="shared" si="0"/>
+        <v>8.815581189928548E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B32" s="11">
+        <v>9</v>
+      </c>
+      <c r="C32" s="4">
+        <v>4031</v>
+      </c>
+      <c r="D32" s="4">
+        <v>0</v>
+      </c>
+      <c r="E32" s="4">
+        <v>0</v>
+      </c>
+      <c r="F32" s="6">
+        <f>C32/$E$23</f>
+        <v>8.8133947858635864E-3</v>
+      </c>
+      <c r="G32" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H32" s="6">
+        <f t="shared" si="3"/>
+        <v>8.8133947858635864E-3</v>
+      </c>
+      <c r="I32" s="1">
+        <f t="shared" si="4"/>
+        <v>0.99975198412698407</v>
+      </c>
+      <c r="J32" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K32" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="2">
+        <f>SUM(C24:C32)</f>
+        <v>10016</v>
+      </c>
+      <c r="D33" s="2">
+        <f>SUM((D24:D32))</f>
+        <v>447839</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" s="7">
+        <f>SUM($F23:$F32)</f>
+        <v>2.1899023114663775E-2</v>
+      </c>
+      <c r="G33" s="7">
+        <f>SUM($G23:$G32)</f>
+        <v>0.97915701004871303</v>
+      </c>
+      <c r="H33" s="7">
+        <f>SUM(H23:H32)</f>
+        <v>1.0010560331633769</v>
+      </c>
+      <c r="I33" s="7">
+        <f>SUM($F23:$F32)</f>
+        <v>2.1899023114663775E-2</v>
+      </c>
+      <c r="J33" s="7">
+        <f>SUM($G23:$G32)</f>
+        <v>0.97915701004871303</v>
+      </c>
+      <c r="K33" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B35E5423-8F9A-4F05-B53B-A434F899C446}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>